<commit_message>
Updates to "Create reference data" - rationalisation
</commit_message>
<xml_diff>
--- a/create-data/create_reference_data/source/additional_code_types.xlsx
+++ b/create-data/create_reference_data/source/additional_code_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\migrate_reference_data\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt.admin/projects/tariffs/create-data/create_reference_data/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95A3F16E-771B-4768-92A6-F731DBD1E25A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFBFD6E-4F5F-7A46-951F-377F7E892341}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="9555" activeTab="1" xr2:uid="{B724F9FD-527C-4A95-969C-B8CCC70DC96A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16180" windowHeight="9560" xr2:uid="{B724F9FD-527C-4A95-969C-B8CCC70DC96A}"/>
   </bookViews>
   <sheets>
     <sheet name="Updated" sheetId="1" r:id="rId1"/>
@@ -26,17 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>DESCRIPTION_OLD</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_NEW</t>
-  </si>
-  <si>
     <t>ADDITIONAL_CODE_TYPE_ID</t>
   </si>
   <si>
@@ -47,9 +41,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>Anti-dumping/countervailing</t>
   </si>
   <si>
     <t>Anti-dumping / anti-subsidy</t>
@@ -442,73 +433,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5B35DA-628F-40A1-97BB-3E7F8D8C3603}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="51.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="30.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.5" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -521,56 +496,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F64BD5-F463-4A11-973E-8749F58C3A6F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="3" max="3" width="19" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>

</xml_diff>